<commit_message>
documentos de errores en excel cargados
</commit_message>
<xml_diff>
--- a/ESEPValidador/data/input/PtoLlerasAgosto.xlsx
+++ b/ESEPValidador/data/input/PtoLlerasAgosto.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wrubios\Documents\.Ejecutables\Correcciones202\08Agosto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wrubios\Documents\.Ejecutables\ESEValidador\ESEPValidador\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB3AA6A-9617-47C0-A4A5-B1204327BC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13A640C-B012-4CD8-B646-33ECD8DE912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="720" windowWidth="14610" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProLlerasAgosto" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ProLlerasAgosto!$A$1:$DO$35</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -4781,9 +4784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87E856A-618A-4DC2-8A6B-7DFD5B8675A2}">
   <dimension ref="A1:DO35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:DO1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5161,7 +5162,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5">
-        <v>168</v>
+        <v>1</v>
       </c>
       <c r="C2" s="6">
         <v>505770063427</v>
@@ -5520,7 +5521,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10">
-        <v>262</v>
+        <v>2</v>
       </c>
       <c r="C3" s="11">
         <v>505770063427</v>
@@ -5879,7 +5880,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="5">
-        <v>554</v>
+        <v>3</v>
       </c>
       <c r="C4" s="6">
         <v>505770063427</v>
@@ -6238,7 +6239,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="10">
-        <v>1064</v>
+        <v>4</v>
       </c>
       <c r="C5" s="11">
         <v>505770063427</v>
@@ -6597,7 +6598,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="5">
-        <v>1274</v>
+        <v>5</v>
       </c>
       <c r="C6" s="6">
         <v>505770063427</v>
@@ -6956,7 +6957,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="10">
-        <v>1441</v>
+        <v>6</v>
       </c>
       <c r="C7" s="11">
         <v>505770063427</v>
@@ -7315,7 +7316,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="5">
-        <v>1561</v>
+        <v>7</v>
       </c>
       <c r="C8" s="6">
         <v>505770063427</v>
@@ -7674,7 +7675,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="10">
-        <v>1597</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11">
         <v>505770063427</v>
@@ -8033,7 +8034,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="5">
-        <v>1793</v>
+        <v>9</v>
       </c>
       <c r="C10" s="6">
         <v>505770063427</v>
@@ -8392,7 +8393,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="10">
-        <v>1969</v>
+        <v>10</v>
       </c>
       <c r="C11" s="11">
         <v>505770063427</v>
@@ -8751,7 +8752,7 @@
         <v>2</v>
       </c>
       <c r="B12" s="5">
-        <v>1972</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6">
         <v>505770063427</v>
@@ -9110,7 +9111,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="10">
-        <v>1980</v>
+        <v>12</v>
       </c>
       <c r="C13" s="11">
         <v>505770063427</v>
@@ -9469,7 +9470,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="5">
-        <v>2612</v>
+        <v>13</v>
       </c>
       <c r="C14" s="6">
         <v>505770063427</v>
@@ -9828,7 +9829,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="10">
-        <v>3017</v>
+        <v>14</v>
       </c>
       <c r="C15" s="11">
         <v>505770063427</v>
@@ -10187,7 +10188,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="5">
-        <v>3040</v>
+        <v>15</v>
       </c>
       <c r="C16" s="6">
         <v>505770063427</v>
@@ -10546,7 +10547,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="10">
-        <v>3579</v>
+        <v>16</v>
       </c>
       <c r="C17" s="11">
         <v>505770063427</v>
@@ -10905,7 +10906,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="5">
-        <v>3600</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6">
         <v>505770063427</v>
@@ -11264,7 +11265,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="10">
-        <v>3873</v>
+        <v>18</v>
       </c>
       <c r="C19" s="11">
         <v>505770063427</v>
@@ -11623,7 +11624,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="5">
-        <v>4083</v>
+        <v>19</v>
       </c>
       <c r="C20" s="6">
         <v>505770063427</v>
@@ -11982,7 +11983,7 @@
         <v>2</v>
       </c>
       <c r="B21" s="10">
-        <v>4505</v>
+        <v>20</v>
       </c>
       <c r="C21" s="11">
         <v>505770063427</v>
@@ -12341,7 +12342,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="5">
-        <v>4552</v>
+        <v>21</v>
       </c>
       <c r="C22" s="6">
         <v>505770063427</v>
@@ -12700,7 +12701,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="10">
-        <v>4891</v>
+        <v>22</v>
       </c>
       <c r="C23" s="11">
         <v>505770063427</v>
@@ -13059,7 +13060,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="5">
-        <v>5021</v>
+        <v>23</v>
       </c>
       <c r="C24" s="6">
         <v>505770063427</v>
@@ -13418,7 +13419,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="10">
-        <v>5267</v>
+        <v>24</v>
       </c>
       <c r="C25" s="11">
         <v>505770063427</v>
@@ -13777,7 +13778,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="5">
-        <v>5286</v>
+        <v>25</v>
       </c>
       <c r="C26" s="6">
         <v>505770063427</v>
@@ -14136,7 +14137,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="10">
-        <v>5443</v>
+        <v>26</v>
       </c>
       <c r="C27" s="11">
         <v>505770063427</v>
@@ -14495,7 +14496,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="5">
-        <v>5486</v>
+        <v>27</v>
       </c>
       <c r="C28" s="6">
         <v>505770063427</v>
@@ -14854,7 +14855,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="10">
-        <v>5487</v>
+        <v>28</v>
       </c>
       <c r="C29" s="11">
         <v>505770063427</v>
@@ -15213,7 +15214,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="5">
-        <v>5490</v>
+        <v>29</v>
       </c>
       <c r="C30" s="6">
         <v>505770063427</v>
@@ -15572,7 +15573,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="10">
-        <v>5494</v>
+        <v>30</v>
       </c>
       <c r="C31" s="11">
         <v>505770063427</v>
@@ -15931,7 +15932,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="5">
-        <v>5496</v>
+        <v>31</v>
       </c>
       <c r="C32" s="6">
         <v>505770063427</v>
@@ -16290,7 +16291,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="10">
-        <v>5501</v>
+        <v>32</v>
       </c>
       <c r="C33" s="11">
         <v>505770063427</v>
@@ -16649,7 +16650,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="5">
-        <v>5502</v>
+        <v>33</v>
       </c>
       <c r="C34" s="6">
         <v>505770063427</v>
@@ -17007,8 +17008,8 @@
       <c r="A35" s="1">
         <v>2</v>
       </c>
-      <c r="B35" s="2">
-        <v>5504</v>
+      <c r="B35" s="10">
+        <v>34</v>
       </c>
       <c r="C35" s="14">
         <v>505770063427</v>
@@ -17363,6 +17364,11 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:DO35" xr:uid="{B87E856A-618A-4DC2-8A6B-7DFD5B8675A2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:DO35">
+      <sortCondition ref="B1:B35"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>